<commit_message>
carte alim maj sch/brd
</commit_message>
<xml_diff>
--- a/datasheet/regulateur_refV/LM2678.xlsx
+++ b/datasheet/regulateur_refV/LM2678.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lucas/Documents/GitHub/RobotMT/datasheet/regulateur_refV/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D07A32-2BE2-7A48-8DCF-69156627A4A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>L</t>
   </si>
@@ -27,24 +33,9 @@
     <t>Code farnel</t>
   </si>
   <si>
-    <t>2333111RL</t>
-  </si>
-  <si>
-    <t>Prix unitaire pour lot de 10</t>
-  </si>
-  <si>
     <t>Cout</t>
   </si>
   <si>
-    <t>1135118RL</t>
-  </si>
-  <si>
-    <t>AVX</t>
-  </si>
-  <si>
-    <t>SPRAGUE</t>
-  </si>
-  <si>
     <t>KEMET</t>
   </si>
   <si>
@@ -63,31 +54,22 @@
     <t>-</t>
   </si>
   <si>
-    <t>pas de stock</t>
-  </si>
-  <si>
     <t>Schottky</t>
   </si>
   <si>
-    <t>1,97*</t>
-  </si>
-  <si>
-    <t>0,573*</t>
-  </si>
-  <si>
-    <t>*Vendu à l'unité</t>
-  </si>
-  <si>
     <t>Through Hole</t>
   </si>
   <si>
-    <t>Coilcraft</t>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Pulse engineering</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -126,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,18 +117,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -195,17 +171,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -236,52 +201,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -316,6 +266,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -640,219 +598,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C2" s="9">
+        <v>2215928</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="C3" s="9">
+        <v>2524603</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11">
+        <v>2424754</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9">
+        <v>9557296</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2287332</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1.6</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="14"/>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2470768</v>
-      </c>
-      <c r="D4" s="6">
-        <v>2.8</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="11"/>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2524603</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1.38</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1.74</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="9"/>
-      <c r="B7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1612263</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="10"/>
-      <c r="B8" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="16">
-        <v>2424754</v>
-      </c>
-      <c r="D8" s="15">
-        <v>1.35</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4">
-        <v>9101330</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1.62</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="11"/>
-      <c r="B10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3">
-        <v>9557296</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A10"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>